<commit_message>
got pipeline finally to work and pushed 202912 through
</commit_message>
<xml_diff>
--- a/metadata/plate_metadata/20250305_well_metadata.xlsx
+++ b/metadata/plate_metadata/20250305_well_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Cole Trapnell's Lab Dropbox/Nick Lammers/Nick/morphseq/metadata/well_metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marazzanocolon/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5472C0A8-942B-F248-8FAB-4599B250DC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8151FBFC-90C8-A64F-8DDE-8CD0419F228D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35400" yWindow="-3420" windowWidth="30240" windowHeight="17080" activeTab="2" xr2:uid="{1D111BDF-EAD8-A94F-AA28-88CC9649B22F}"/>
+    <workbookView xWindow="1040" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="8" xr2:uid="{1D111BDF-EAD8-A94F-AA28-88CC9649B22F}"/>
   </bookViews>
   <sheets>
     <sheet name="medium" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="series_number_map" sheetId="9" r:id="rId6"/>
     <sheet name="start_age_morph" sheetId="8" r:id="rId7"/>
     <sheet name="embryos_per_well" sheetId="7" r:id="rId8"/>
+    <sheet name="temperature" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -81,23 +82,23 @@
     <t>MC05</t>
   </si>
   <si>
-    <t>cep290_het</t>
+    <t>cep290_heterozygous</t>
   </si>
   <si>
-    <t>wildtype</t>
+    <t>cep290_homozygous</t>
   </si>
   <si>
-    <t>unknown</t>
+    <t>cep290_unknown</t>
   </si>
   <si>
-    <t>cep290_homo</t>
+    <t>cep290_wildtype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +119,18 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,16 +149,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{53658B1D-257B-3945-9C20-976A5F19BE65}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1221,11 +1238,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77E54D0-3682-084C-87D6-317C30F3BB42}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -1276,7 +1302,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
@@ -1285,22 +1311,22 @@
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>12</v>
@@ -1314,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -1323,28 +1349,28 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1367,22 +1393,22 @@
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>12</v>
@@ -1393,16 +1419,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -1423,10 +1449,10 @@
         <v>14</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1437,13 +1463,13 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>14</v>
@@ -1452,7 +1478,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>12</v>
@@ -1467,7 +1493,7 @@
         <v>14</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1475,22 +1501,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>12</v>
@@ -1502,13 +1528,13 @@
         <v>14</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1519,14 +1545,14 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1537,10 +1563,10 @@
         <v>12</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>12</v>
@@ -1549,7 +1575,7 @@
         <v>12</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1557,10 +1583,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
@@ -1578,19 +1604,19 @@
         <v>12</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2738,7 +2764,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2917,4 +2943,389 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BC51DA-2B79-A14A-B73A-E336F2529846}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4">
+        <v>30</v>
+      </c>
+      <c r="H2" s="4">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4">
+        <v>30</v>
+      </c>
+      <c r="K2" s="4">
+        <v>30</v>
+      </c>
+      <c r="L2" s="4">
+        <v>30</v>
+      </c>
+      <c r="M2" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4">
+        <v>30</v>
+      </c>
+      <c r="H3" s="4">
+        <v>30</v>
+      </c>
+      <c r="I3" s="4">
+        <v>30</v>
+      </c>
+      <c r="J3" s="4">
+        <v>30</v>
+      </c>
+      <c r="K3" s="4">
+        <v>30</v>
+      </c>
+      <c r="L3" s="4">
+        <v>30</v>
+      </c>
+      <c r="M3" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4">
+        <v>30</v>
+      </c>
+      <c r="G4" s="4">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4">
+        <v>30</v>
+      </c>
+      <c r="J4" s="4">
+        <v>30</v>
+      </c>
+      <c r="K4" s="4">
+        <v>30</v>
+      </c>
+      <c r="L4" s="4">
+        <v>30</v>
+      </c>
+      <c r="M4" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4">
+        <v>30</v>
+      </c>
+      <c r="D5" s="4">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4">
+        <v>30</v>
+      </c>
+      <c r="H5" s="4">
+        <v>30</v>
+      </c>
+      <c r="I5" s="4">
+        <v>30</v>
+      </c>
+      <c r="J5" s="4">
+        <v>30</v>
+      </c>
+      <c r="K5" s="4">
+        <v>30</v>
+      </c>
+      <c r="L5" s="4">
+        <v>30</v>
+      </c>
+      <c r="M5" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4">
+        <v>30</v>
+      </c>
+      <c r="H6" s="4">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4">
+        <v>30</v>
+      </c>
+      <c r="J6" s="4">
+        <v>30</v>
+      </c>
+      <c r="K6" s="4">
+        <v>30</v>
+      </c>
+      <c r="L6" s="4">
+        <v>30</v>
+      </c>
+      <c r="M6" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4">
+        <v>30</v>
+      </c>
+      <c r="G7" s="4">
+        <v>30</v>
+      </c>
+      <c r="H7" s="4">
+        <v>30</v>
+      </c>
+      <c r="I7" s="4">
+        <v>30</v>
+      </c>
+      <c r="J7" s="4">
+        <v>30</v>
+      </c>
+      <c r="K7" s="4">
+        <v>30</v>
+      </c>
+      <c r="L7" s="4">
+        <v>30</v>
+      </c>
+      <c r="M7" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4">
+        <v>30</v>
+      </c>
+      <c r="F8" s="4">
+        <v>30</v>
+      </c>
+      <c r="G8" s="4">
+        <v>30</v>
+      </c>
+      <c r="H8" s="4">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4">
+        <v>30</v>
+      </c>
+      <c r="J8" s="4">
+        <v>30</v>
+      </c>
+      <c r="K8" s="4">
+        <v>30</v>
+      </c>
+      <c r="L8" s="4">
+        <v>30</v>
+      </c>
+      <c r="M8" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4">
+        <v>30</v>
+      </c>
+      <c r="G9" s="4">
+        <v>30</v>
+      </c>
+      <c r="H9" s="4">
+        <v>30</v>
+      </c>
+      <c r="I9" s="4">
+        <v>30</v>
+      </c>
+      <c r="J9" s="4">
+        <v>30</v>
+      </c>
+      <c r="K9" s="4">
+        <v>30</v>
+      </c>
+      <c r="L9" s="4">
+        <v>30</v>
+      </c>
+      <c r="M9" s="4">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>